<commit_message>
Possibilidade de recalcular as métricas com os dados salvos em pkl.
Signed-off-by: Ariel Tadeu da Silva <silva.ariel2013@gmail.com>
</commit_message>
<xml_diff>
--- a/main/results/tables/adult.xlsx
+++ b/main/results/tables/adult.xlsx
@@ -485,177 +485,177 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>cruds</t>
+          <t>cem</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>4.17</v>
+        <v>5.77</v>
       </c>
       <c r="D3" t="n">
-        <v>2.267905295237643</v>
+        <v>0.9154653998284462</v>
       </c>
       <c r="E3" t="n">
-        <v>1.911294723527047</v>
+        <v>0.8401729275609791</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4478978382746379</v>
+        <v>0.8349427956342698</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>cchvae</t>
+          <t>wachter</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>9.59</v>
+        <v>3.75</v>
       </c>
       <c r="D4" t="n">
-        <v>4.288725759924322</v>
+        <v>0.4935082787960795</v>
       </c>
       <c r="E4" t="n">
-        <v>3.718921594863702</v>
+        <v>0.3940633180178528</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9920547244320177</v>
+        <v>0.3940707594163054</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>clue</t>
+          <t>face-epsilon</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="C5" t="n">
-        <v>8.65</v>
+        <v>7.47</v>
       </c>
       <c r="D5" t="n">
-        <v>3.454601607651509</v>
+        <v>3.952951915305309</v>
       </c>
       <c r="E5" t="n">
-        <v>2.811658536566437</v>
+        <v>3.475175654078315</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9927476534247398</v>
+        <v>0.9432876712328766</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>ar</t>
+          <t>cchvae</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.26</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.55</v>
+        <v>9.59</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4004687407569555</v>
+        <v>4.288725759924322</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4000020792020286</v>
+        <v>3.718921594863702</v>
       </c>
       <c r="F6" t="n">
-        <v>0.26</v>
+        <v>0.9920547244320177</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>wachter</t>
+          <t>ar</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="C7" t="n">
-        <v>3.75</v>
+        <v>0.55</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4935082787960795</v>
+        <v>0.4004687407569555</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3940633180178528</v>
+        <v>0.4000020792020286</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3940707594163054</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>dice</t>
+          <t>cruds</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="C8" t="n">
-        <v>2.39</v>
+        <v>4.17</v>
       </c>
       <c r="D8" t="n">
-        <v>1.748663095629701</v>
+        <v>2.267905295237643</v>
       </c>
       <c r="E8" t="n">
-        <v>1.521672553600215</v>
+        <v>1.911294723527047</v>
       </c>
       <c r="F8" t="n">
-        <v>0.923548830246621</v>
+        <v>0.4478978382746379</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>gs</t>
+          <t>face-knn</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>6.17</v>
+        <v>8.08</v>
       </c>
       <c r="D9" t="n">
-        <v>1.366335199349296</v>
+        <v>4.312361890239652</v>
       </c>
       <c r="E9" t="n">
-        <v>1.184234398993123</v>
+        <v>3.830199795020054</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8371560574946735</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>cem</t>
+          <t>clue</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>5.77</v>
+        <v>8.65</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9154653998284462</v>
+        <v>3.454601607651509</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8401729275609791</v>
+        <v>2.811658536566437</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8349427956342698</v>
+        <v>0.9927476534247398</v>
       </c>
     </row>
     <row r="11">
@@ -683,45 +683,45 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>face-epsilon</t>
+          <t>gs</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>7.47</v>
+        <v>6.17</v>
       </c>
       <c r="D12" t="n">
-        <v>3.952951915305309</v>
+        <v>1.366335199349296</v>
       </c>
       <c r="E12" t="n">
-        <v>3.475175654078315</v>
+        <v>1.184234398993123</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9432876712328766</v>
+        <v>0.8371560574946735</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>face-knn</t>
+          <t>dice</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>8.08</v>
+        <v>2.39</v>
       </c>
       <c r="D13" t="n">
-        <v>4.312361890239652</v>
+        <v>1.748663095629701</v>
       </c>
       <c r="E13" t="n">
-        <v>3.830199795020054</v>
+        <v>1.521672553600215</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0.923548830246621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX — CERScore como inverso da distância. Recalculados valores.
Signed-off-by: Ariel Tadeu da Silva <silva.ariel2013@gmail.com>
</commit_message>
<xml_diff>
--- a/main/results/tables/adult.xlsx
+++ b/main/results/tables/adult.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,243 +485,199 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>cem</t>
+          <t>face-knn</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>5.77</v>
+        <v>9.835418325367966</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9154653998284462</v>
+        <v>21.95489729689547</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8401729275609791</v>
+        <v>26.503318857581</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8349427956342698</v>
+        <v>75.60882951000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>wachter</t>
+          <t>dice</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>3.75</v>
+        <v>40.91807604500001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4935082787960795</v>
+        <v>76.92589078860948</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3940633180178528</v>
+        <v>215.1916095887813</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3940707594163054</v>
+        <v>111.2721740379802</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>face-epsilon</t>
+          <t>clue</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>7.47</v>
+        <v>10.82941470457071</v>
       </c>
       <c r="D5" t="n">
-        <v>3.952951915305309</v>
+        <v>34.294330352762</v>
       </c>
       <c r="E5" t="n">
-        <v>3.475175654078315</v>
+        <v>61.15496029938544</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9432876712328766</v>
+        <v>96.242649608826</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>cchvae</t>
+          <t>cruds</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="C6" t="n">
-        <v>9.59</v>
+        <v>2.502678916033189</v>
       </c>
       <c r="D6" t="n">
-        <v>4.288725759924322</v>
+        <v>5.233592245180635</v>
       </c>
       <c r="E6" t="n">
-        <v>3.718921594863702</v>
+        <v>6.850932417469378</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9920547244320177</v>
+        <v>21.91949592025048</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>ar</t>
+          <t>cem</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.26</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.55</v>
+        <v>10.32785084621429</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4004687407569555</v>
+        <v>490.2476918543464</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4000020792020286</v>
+        <v>25698.92363656488</v>
       </c>
       <c r="F7" t="n">
-        <v>0.26</v>
+        <v>494.5480324535401</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>cruds</t>
+          <t>wachter</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.45</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>4.17</v>
+        <v>2.801242255</v>
       </c>
       <c r="D8" t="n">
-        <v>2.267905295237643</v>
+        <v>77.04564214242079</v>
       </c>
       <c r="E8" t="n">
-        <v>1.911294723527047</v>
+        <v>5008.075595881454</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4478978382746379</v>
+        <v>414.1865435513668</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>face-knn</t>
+          <t>face-epsilon</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="C9" t="n">
-        <v>8.08</v>
+        <v>8.808593235964647</v>
       </c>
       <c r="D9" t="n">
-        <v>4.312361890239652</v>
+        <v>18.9142653180085</v>
       </c>
       <c r="E9" t="n">
-        <v>3.830199795020054</v>
+        <v>22.28621378253619</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>64.9514995</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>clue</t>
+          <t>gs</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>8.65</v>
+        <v>10.56844646036905</v>
       </c>
       <c r="D10" t="n">
-        <v>3.454601607651509</v>
+        <v>128.4959148244709</v>
       </c>
       <c r="E10" t="n">
-        <v>2.811658536566437</v>
+        <v>5405.51302451188</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9927476534247398</v>
+        <v>305.8624585226183</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>cem-vae</t>
+          <t>ar</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0.26</v>
       </c>
       <c r="C11" t="n">
-        <v>5.77</v>
+        <v>2.91803754</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9152786894707802</v>
+        <v>3.965654871881759</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8401227542653745</v>
+        <v>3.979414772917486</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8349162352085113</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>gs</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>6.17</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1.366335199349296</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1.184234398993123</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.8371560574946735</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>dice</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2.39</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1.748663095629701</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1.521672553600215</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.923548830246621</v>
+        <v>4.96790886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>